<commit_message>
Death's Door + readmeak zuzendu
</commit_message>
<xml_diff>
--- a/Death's Door/DeathsDoor_EU.xlsx
+++ b/Death's Door/DeathsDoor_EU.xlsx
@@ -1315,7 +1315,7 @@
 [sound][anim]Don't worry,[pause] I'll put your ashes in a lovely urn.</t>
   </si>
   <si>
-    <t xml:space="preserve">[sound]Gu biok gauza bat dugu berdina, bele txikia...
+    <t xml:space="preserve">[sound]Guk biok gauza bat dugu berdina, bele txikia...
 Bai, [i]nagusi[/] bera daukagu...
 [anim]Baina, demontre, ezin diogu ikusi duzun guztia berari kontatu.
 [sound][anim]Ez arduratu,[pause] ontzi polit-polit bat bilatuko dut zure errautsentzat.</t>
@@ -17273,8 +17273,8 @@
   </sheetPr>
   <dimension ref="A1:H933"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A462" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C466" activeCellId="0" sqref="C466"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19079,14 +19079,14 @@
       </c>
       <c r="F59" s="9" t="str">
         <f aca="false">IF(ISBLANK(C59),D59,C59)</f>
-        <v>[sound]Gu biok gauza bat dugu berdina, bele txikia...
+        <v>[sound]Guk biok gauza bat dugu berdina, bele txikia...
 Bai, [i]nagusi[/] bera daukagu...
 [anim]Baina, demontre, ezin diogu ikusi duzun guztia berari kontatu.
 [sound][anim]Ez arduratu,[pause] ontzi polit-polit bat bilatuko dut zure errautsentzat.</v>
       </c>
       <c r="G59" s="9" t="str">
         <f aca="false">IF(ISBLANK(C59),E59,C59)</f>
-        <v>[sound]Gu biok gauza bat dugu berdina, bele txikia...
+        <v>[sound]Guk biok gauza bat dugu berdina, bele txikia...
 Bai, [i]nagusi[/] bera daukagu...
 [anim]Baina, demontre, ezin diogu ikusi duzun guztia berari kontatu.
 [sound][anim]Ez arduratu,[pause] ontzi polit-polit bat bilatuko dut zure errautsentzat.</v>

</xml_diff>

<commit_message>
Death's Door - zuzenketak
</commit_message>
<xml_diff>
--- a/Death's Door/DeathsDoor_EU.xlsx
+++ b/Death's Door/DeathsDoor_EU.xlsx
@@ -1285,7 +1285,7 @@
 I can fool the &lt;i&gt;Grim Reaper&lt;/i&gt; himself!</t>
   </si>
   <si>
-    <t xml:space="preserve">Ipurbeltz madarikatua.
+    <t xml:space="preserve">Ipurbeltz madarikatua!
 Beleek ez dute inoiz obeditzen...
 [anim]Biziak salbatu nahian nabil, aizu!
 Ez al duzu ulertzen? &lt;i&gt;Heriok&lt;/i&gt; ez ditu ikusten haien bizi-indarra errautsontzi batean ezkutatzen duten horiek!
@@ -1353,7 +1353,7 @@
 Zeramikaren aztia, [beat]Lurrontzien belagilea, [beat]Lapikoen atsoa...
 Eta -[pause] jakina -[pause] Amona.
 [camera]Ama-senak bultzaturik,[beat] eta Heriori iruzur egiteko ahaleginek itsuturik, bere bizitza pasioz bete zuen: pasioa magiarekiko,[beat] erreanimazioarekiko,[beat] edabeekiko...
-[ANIM][camera]eta lapikoekiko...
+[ANIM][camera]...eta lapikoekiko...
 [camera][ANIM]Amaitu da bere bidaia,[beat] eta orain bakean datza.
 [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina.
 Agortu da mundu honetan zeukan denbora.</t>
@@ -1391,7 +1391,7 @@
   </si>
   <si>
     <t xml:space="preserve">Bizi zen bezala hil da...
-...buruan lapiko bat zuela.</t>
+...errautsontzi bati lotuta.</t>
   </si>
   <si>
     <t xml:space="preserve">Murió tal como vivió...
@@ -1595,7 +1595,7 @@
   </si>
   <si>
     <t xml:space="preserve">Ezin zaitut lagundu esleitu zaizun arima ekartzen ez badidazu!
-Ez duzu ikusten zein estresatua nagoen!?</t>
+Ez duzu ikusten zeinen estresatua nagoen!?</t>
   </si>
   <si>
     <t xml:space="preserve">¡No puedo ayudarte a menos que traigas el alma asignada!
@@ -1624,7 +1624,7 @@
 Sentitzen dut, [beat]baina oihanak berak itxi zituen ziegetarako ateak orain dela ilargi asko, gu babesteko asmoz.
 Berekin hitz egin nezake, [beat]eta agian zuretzako ateak ireki ditzan konbentzitu...
 Baina, [beat]gure elkarrizketak abesti bidezkoak dira,[beat] eta zoritxarrez...
-[sound][anim]nire adar magikoa galdu dut...
+[sound][anim]...nire adar magikoa galdu dut...
 Iparraldeko kanpamendu zaharrean utzi nuen. Tamalez, Igel Erregearen morroiek kanporatu gintuzten.
 Adarra itzultzen badidazu,[beat] ziur naiz zure bidaian lagundu ahalko zaitugula.</t>
   </si>
@@ -2010,7 +2010,7 @@
   </si>
   <si>
     <t xml:space="preserve">[speed40]Gaur hemen batu gara Igel Erregearen heriotza negartzeko.
-[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen, betidanik zeukan amets huts bategatik: oihan osoa ezarri nahi zuen bere agindupean.
+[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen betidanik izan zuen amets soil bategatik: oihan osoa ezarri nahi zuen bere agindupean.
 [ANIM][camera]Eta, [BEAT]noizbehinka,[PAUSE] bere ipurdipean ere bai.
 [camera][ANIM]Amaitu da bere agintaldia, eta zingira osoak nabarituko du bere hutsa. [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina. Agortu da mundu honetan zeukan denbora.</t>
   </si>
@@ -2063,7 +2063,7 @@
 [anim]If only I could &lt;i&gt;smash up&lt;/i&gt; these blasted rocks blocking the path...</t>
   </si>
   <si>
-    <t xml:space="preserve">Ongi etorri,[beat] bidaiariai!
+    <t xml:space="preserve">Ongi etorri,[beat] bidaiaria!
 Aurrera, bota - nola doa zure abentura?
 [anim]Baduzu istorio zirraragarririk, bertatik kantu bat sor dezadan?
 Izan ere, mendi goi hauetara nire hurrengo maisulanarentzako inspirazio bila etorri naiz...
@@ -4771,7 +4771,7 @@
   </si>
   <si>
     <t xml:space="preserve">O, ikusten dut bulego sail zaharrak arakatzen aritu zarela.
-Ekialdeko atalean lan egiten nuen nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
+Ekialdeko atalean lan egiten nuen, nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
 Orain askoz zoriontsuagoa naiz,[beat] baina bulegoa benetan ederra zen!</t>
   </si>
   <si>
@@ -4863,7 +4863,7 @@
   </si>
   <si>
     <t xml:space="preserve">Esadazu...[pause] Ikusi duzu inoiz
-&lt;i&gt;mendirik&lt;/i&gt;?
+...&lt;i&gt;mendirik&lt;/i&gt;?
 Inoiz aukerarik baduzu,[beat] arakatu mendi baten inguruak...
 Zeinen sorkuntza zoragarria diren,[break] naturako titanak!</t>
   </si>
@@ -6632,7 +6632,7 @@
   <si>
     <t xml:space="preserve">Txutxumutxu bat entzun dut...[pause] bele bati buruz, orain dela urte asko,[beat] eta asko...
 Bele honek ez zuen bere egitekoa burutzerik izan, eta bere atea &lt;i&gt;eskuz&lt;/i&gt; kendu behar izan zuten, biltegian gordetzeko!
-Diotenez egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
+Diotenez, egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
 &lt;i&gt;Hiru&lt;/i&gt; mekanografo zorabiatu ziren nekearen nekez!
 Oh, zer inbidia ematen didaten...</t>
   </si>
@@ -6658,7 +6658,7 @@
 That would be amazing!</t>
   </si>
   <si>
-    <t xml:space="preserve">Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko ditut izapide pilo erraldoi bat...
+    <t xml:space="preserve">Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko dut izapide pilo erraldoi bat...
 Zoragarria litzateke!</t>
   </si>
   <si>
@@ -9120,7 +9120,7 @@
   </si>
   <si>
     <t xml:space="preserve">Honek segari baten eguneroko abandonatua dirudi:
-“Ate ireki batzuk deskonektatzeko agindu digute, energia gainkarga ezohikoa antzeman zen ingurukoak dira.
+“Ate ireki batzuk deskonektatzeko agindu digute. Energia gainkarga ezohikoa antzeman zen ingurukoak dira.
 Zonalde hori nahiko aktiboa zen lehen, Komisioko kideek &lt;i&gt;sorgina&lt;/i&gt; bere ikerketan laguntzeko erabiltzen baitzuten.
 Agindua eman bezain laster bete denez, ez dakit zer gertatu zaien bertan zeuden beleei...
 Oraingoz, ate guztiak zigilatu dira, eta burutu gabe zeuden bertako lan-aginduak eskuz itxi dira.
@@ -9988,7 +9988,7 @@
 It seems she may have had to remove it because of her constantly swelling body. Such are the risks of living beyond your years.</t>
   </si>
   <si>
-    <t xml:space="preserve">Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia, zu arrautza zinen garaia baino zaharragoa da.
+    <t xml:space="preserve">Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia da, zu arrautza zinen garaia baino zaharragoa.
 Badirudi sorginak kendu beharra izan zuela, gorputza etengabe puzten ari zitzaiolako. Hori ere zure garaia igarota bizitzen jarraitzearen ondorioetako bat da.</t>
   </si>
   <si>
@@ -10662,7 +10662,7 @@
 In the right hands, this instrument can create a dialogue with nature, allowing some degree of control over nearby plant life.</t>
   </si>
   <si>
-    <t xml:space="preserve">Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere Oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
+    <t xml:space="preserve">Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere, oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
 Esku egokietan, instrumentu honek naturarekin elkarrizketa bat sor dezake, inguruko landaretza nolabait kontrolatzea ahalbidetuz.</t>
   </si>
   <si>
@@ -10890,7 +10890,7 @@
   </si>
   <si>
     <t xml:space="preserve">Eskalara egindako atearen maketa honek ohar bat dauka itsatsita:
-&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrak bezala.
+&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrekoek bezala.
 Ganbera korazatu bat aurkeztuko dugu, ate berrientzako argindar-sarea elikatzeko arimak prozesatuko dituena.
 Guztia Komisioak automatizatua egongo da, erosketak egiteko erabiltzen diren arima txikiak ere sistema berrelikatzeko erabiliko dira.”&lt;/i&gt;</t>
   </si>
@@ -17273,14 +17273,14 @@
   </sheetPr>
   <dimension ref="A1:H933"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G402" activeCellId="0" sqref="G402:G669"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E117" activeCellId="0" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="51.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="42.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="43.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="25.51"/>
@@ -19045,7 +19045,7 @@
       </c>
       <c r="F58" s="9" t="str">
         <f aca="false">IF(ISBLANK(C58),D58,C58)</f>
-        <v>Ipurbeltz madarikatua.
+        <v>Ipurbeltz madarikatua!
 Beleek ez dute inoiz obeditzen...
 [anim]Biziak salbatu nahian nabil, aizu!
 Ez al duzu ulertzen? &lt;i&gt;Heriok&lt;/i&gt; ez ditu ikusten haien bizi-indarra errautsontzi batean ezkutatzen duten horiek!
@@ -19053,7 +19053,7 @@
       </c>
       <c r="G58" s="9" t="str">
         <f aca="false">IF(ISBLANK(C58),E58,C58)</f>
-        <v>Ipurbeltz madarikatua.
+        <v>Ipurbeltz madarikatua!
 Beleek ez dute inoiz obeditzen...
 [anim]Biziak salbatu nahian nabil, aizu!
 Ez al duzu ulertzen? &lt;i&gt;Heriok&lt;/i&gt; ez ditu ikusten haien bizi-indarra errautsontzi batean ezkutatzen duten horiek!
@@ -19116,7 +19116,7 @@
 Zeramikaren aztia, [beat]Lurrontzien belagilea, [beat]Lapikoen atsoa...
 Eta -[pause] jakina -[pause] Amona.
 [camera]Ama-senak bultzaturik,[beat] eta Heriori iruzur egiteko ahaleginek itsuturik, bere bizitza pasioz bete zuen: pasioa magiarekiko,[beat] erreanimazioarekiko,[beat] edabeekiko...
-[ANIM][camera]eta lapikoekiko...
+[ANIM][camera]...eta lapikoekiko...
 [camera][ANIM]Amaitu da bere bidaia,[beat] eta orain bakean datza.
 [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina.
 Agortu da mundu honetan zeukan denbora.</v>
@@ -19128,7 +19128,7 @@
 Zeramikaren aztia, [beat]Lurrontzien belagilea, [beat]Lapikoen atsoa...
 Eta -[pause] jakina -[pause] Amona.
 [camera]Ama-senak bultzaturik,[beat] eta Heriori iruzur egiteko ahaleginek itsuturik, bere bizitza pasioz bete zuen: pasioa magiarekiko,[beat] erreanimazioarekiko,[beat] edabeekiko...
-[ANIM][camera]eta lapikoekiko...
+[ANIM][camera]...eta lapikoekiko...
 [camera][ANIM]Amaitu da bere bidaia,[beat] eta orain bakean datza.
 [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina.
 Agortu da mundu honetan zeukan denbora.</v>
@@ -19154,12 +19154,12 @@
       <c r="F61" s="9" t="str">
         <f aca="false">IF(ISBLANK(C61),D61,C61)</f>
         <v>Bizi zen bezala hil da...
-...buruan lapiko bat zuela.</v>
+...errautsontzi bati lotuta.</v>
       </c>
       <c r="G61" s="9" t="str">
         <f aca="false">IF(ISBLANK(C61),E61,C61)</f>
         <v>Bizi zen bezala hil da...
-...buruan lapiko bat zuela.</v>
+...errautsontzi bati lotuta.</v>
       </c>
       <c r="H61" s="5"/>
     </row>
@@ -19412,12 +19412,12 @@
       <c r="F69" s="9" t="str">
         <f aca="false">IF(ISBLANK(C69),D69,C69)</f>
         <v>Ezin zaitut lagundu esleitu zaizun arima ekartzen ez badidazu!
-Ez duzu ikusten zein estresatua nagoen!?</v>
+Ez duzu ikusten zeinen estresatua nagoen!?</v>
       </c>
       <c r="G69" s="9" t="str">
         <f aca="false">IF(ISBLANK(C69),E69,C69)</f>
         <v>Ezin zaitut lagundu esleitu zaizun arima ekartzen ez badidazu!
-Ez duzu ikusten zein estresatua nagoen!?</v>
+Ez duzu ikusten zeinen estresatua nagoen!?</v>
       </c>
       <c r="H69" s="5"/>
     </row>
@@ -19444,7 +19444,7 @@
 Sentitzen dut, [beat]baina oihanak berak itxi zituen ziegetarako ateak orain dela ilargi asko, gu babesteko asmoz.
 Berekin hitz egin nezake, [beat]eta agian zuretzako ateak ireki ditzan konbentzitu...
 Baina, [beat]gure elkarrizketak abesti bidezkoak dira,[beat] eta zoritxarrez...
-[sound][anim]nire adar magikoa galdu dut...
+[sound][anim]...nire adar magikoa galdu dut...
 Iparraldeko kanpamendu zaharrean utzi nuen. Tamalez, Igel Erregearen morroiek kanporatu gintuzten.
 Adarra itzultzen badidazu,[beat] ziur naiz zure bidaian lagundu ahalko zaitugula.</v>
       </c>
@@ -19455,7 +19455,7 @@
 Sentitzen dut, [beat]baina oihanak berak itxi zituen ziegetarako ateak orain dela ilargi asko, gu babesteko asmoz.
 Berekin hitz egin nezake, [beat]eta agian zuretzako ateak ireki ditzan konbentzitu...
 Baina, [beat]gure elkarrizketak abesti bidezkoak dira,[beat] eta zoritxarrez...
-[sound][anim]nire adar magikoa galdu dut...
+[sound][anim]...nire adar magikoa galdu dut...
 Iparraldeko kanpamendu zaharrean utzi nuen. Tamalez, Igel Erregearen morroiek kanporatu gintuzten.
 Adarra itzultzen badidazu,[beat] ziur naiz zure bidaian lagundu ahalko zaitugula.</v>
       </c>
@@ -19920,14 +19920,14 @@
       <c r="F85" s="9" t="str">
         <f aca="false">IF(ISBLANK(C85),D85,C85)</f>
         <v>[speed40]Gaur hemen batu gara Igel Erregearen heriotza negartzeko.
-[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen, betidanik zeukan amets huts bategatik: oihan osoa ezarri nahi zuen bere agindupean.
+[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen betidanik izan zuen amets soil bategatik: oihan osoa ezarri nahi zuen bere agindupean.
 [ANIM][camera]Eta, [BEAT]noizbehinka,[PAUSE] bere ipurdipean ere bai.
 [camera][ANIM]Amaitu da bere agintaldia, eta zingira osoak nabarituko du bere hutsa. [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina. Agortu da mundu honetan zeukan denbora.</v>
       </c>
       <c r="G85" s="9" t="str">
         <f aca="false">IF(ISBLANK(C85),E85,C85)</f>
         <v>[speed40]Gaur hemen batu gara Igel Erregearen heriotza negartzeko.
-[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen, betidanik zeukan amets huts bategatik: oihan osoa ezarri nahi zuen bere agindupean.
+[camera]Buruzagi sendoa eta beldurrezina,[BEAT] jazarria izan zen betidanik izan zuen amets soil bategatik: oihan osoa ezarri nahi zuen bere agindupean.
 [ANIM][camera]Eta, [BEAT]noizbehinka,[PAUSE] bere ipurdipean ere bai.
 [camera][ANIM]Amaitu da bere agintaldia, eta zingira osoak nabarituko du bere hutsa. [ANIM]Makurtu burua bere omenez. [PAUSE]Erakutsi dolumina. Agortu da mundu honetan zeukan denbora.</v>
       </c>
@@ -19979,7 +19979,7 @@
       </c>
       <c r="F87" s="9" t="str">
         <f aca="false">IF(ISBLANK(C87),D87,C87)</f>
-        <v>Ongi etorri,[beat] bidaiariai!
+        <v>Ongi etorri,[beat] bidaiaria!
 Aurrera, bota - nola doa zure abentura?
 [anim]Baduzu istorio zirraragarririk, bertatik kantu bat sor dezadan?
 Izan ere, mendi goi hauetara nire hurrengo maisulanarentzako inspirazio bila etorri naiz...
@@ -19990,7 +19990,7 @@
       </c>
       <c r="G87" s="9" t="str">
         <f aca="false">IF(ISBLANK(C87),E87,C87)</f>
-        <v>Ongi etorri,[beat] bidaiariai!
+        <v>Ongi etorri,[beat] bidaiaria!
 Aurrera, bota - nola doa zure abentura?
 [anim]Baduzu istorio zirraragarririk, bertatik kantu bat sor dezadan?
 Izan ere, mendi goi hauetara nire hurrengo maisulanarentzako inspirazio bila etorri naiz...
@@ -23666,13 +23666,13 @@
       <c r="F212" s="9" t="str">
         <f aca="false">IF(ISBLANK(C212),D212,C212)</f>
         <v>O, ikusten dut bulego sail zaharrak arakatzen aritu zarela.
-Ekialdeko atalean lan egiten nuen nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
+Ekialdeko atalean lan egiten nuen, nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
 Orain askoz zoriontsuagoa naiz,[beat] baina bulegoa benetan ederra zen!</v>
       </c>
       <c r="G212" s="9" t="str">
         <f aca="false">IF(ISBLANK(C212),E212,C212)</f>
         <v>O, ikusten dut bulego sail zaharrak arakatzen aritu zarela.
-Ekialdeko atalean lan egiten nuen nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
+Ekialdeko atalean lan egiten nuen, nire Benetako Bizitza besarkatu eta lehia burugabe hura utzi nuen arte.
 Orain askoz zoriontsuagoa naiz,[beat] baina bulegoa benetan ederra zen!</v>
       </c>
       <c r="H212" s="5"/>
@@ -23786,14 +23786,14 @@
       <c r="F216" s="9" t="str">
         <f aca="false">IF(ISBLANK(C216),D216,C216)</f>
         <v>Esadazu...[pause] Ikusi duzu inoiz
-&lt;i&gt;mendirik&lt;/i&gt;?
+...&lt;i&gt;mendirik&lt;/i&gt;?
 Inoiz aukerarik baduzu,[beat] arakatu mendi baten inguruak...
 Zeinen sorkuntza zoragarria diren,[break] naturako titanak!</v>
       </c>
       <c r="G216" s="9" t="str">
         <f aca="false">IF(ISBLANK(C216),E216,C216)</f>
         <v>Esadazu...[pause] Ikusi duzu inoiz
-&lt;i&gt;mendirik&lt;/i&gt;?
+...&lt;i&gt;mendirik&lt;/i&gt;?
 Inoiz aukerarik baduzu,[beat] arakatu mendi baten inguruak...
 Zeinen sorkuntza zoragarria diren,[break] naturako titanak!</v>
       </c>
@@ -26233,7 +26233,7 @@
         <f aca="false">IF(ISBLANK(C300),D300,C300)</f>
         <v>Txutxumutxu bat entzun dut...[pause] bele bati buruz, orain dela urte asko,[beat] eta asko...
 Bele honek ez zuen bere egitekoa burutzerik izan, eta bere atea &lt;i&gt;eskuz&lt;/i&gt; kendu behar izan zuten, biltegian gordetzeko!
-Diotenez egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
+Diotenez, egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
 &lt;i&gt;Hiru&lt;/i&gt; mekanografo zorabiatu ziren nekearen nekez!
 Oh, zer inbidia ematen didaten...</v>
       </c>
@@ -26241,7 +26241,7 @@
         <f aca="false">IF(ISBLANK(C300),E300,C300)</f>
         <v>Txutxumutxu bat entzun dut...[pause] bele bati buruz, orain dela urte asko,[beat] eta asko...
 Bele honek ez zuen bere egitekoa burutzerik izan, eta bere atea &lt;i&gt;eskuz&lt;/i&gt; kendu behar izan zuten, biltegian gordetzeko!
-Diotenez egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
+Diotenez, egin beharreko izapideak ordura arte inoiz ikusi gabeak izan ziren![beat] Inprimaki &lt;i&gt;berriak&lt;/i&gt; asmatu behar izan zituzten!
 &lt;i&gt;Hiru&lt;/i&gt; mekanografo zorabiatu ziren nekearen nekez!
 Oh, zer inbidia ematen didaten...</v>
       </c>
@@ -26265,12 +26265,12 @@
       </c>
       <c r="F301" s="9" t="str">
         <f aca="false">IF(ISBLANK(C301),D301,C301)</f>
-        <v>Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko ditut izapide pilo erraldoi bat...
+        <v>Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko dut izapide pilo erraldoi bat...
 Zoragarria litzateke!</v>
       </c>
       <c r="G301" s="9" t="str">
         <f aca="false">IF(ISBLANK(C301),E301,C301)</f>
-        <v>Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko ditut izapide pilo erraldoi bat...
+        <v>Egiteko hau burutu aurretik hiltzen bazara, agian &lt;i&gt;nik&lt;/i&gt; ere bete beharko dut izapide pilo erraldoi bat...
 Zoragarria litzateke!</v>
       </c>
       <c r="H301" s="5"/>
@@ -29840,7 +29840,7 @@
       <c r="F426" s="9" t="str">
         <f aca="false">IF(ISBLANK(C426),D426,C426)</f>
         <v>Honek segari baten eguneroko abandonatua dirudi:
-“Ate ireki batzuk deskonektatzeko agindu digute, energia gainkarga ezohikoa antzeman zen ingurukoak dira.
+“Ate ireki batzuk deskonektatzeko agindu digute. Energia gainkarga ezohikoa antzeman zen ingurukoak dira.
 Zonalde hori nahiko aktiboa zen lehen, Komisioko kideek &lt;i&gt;sorgina&lt;/i&gt; bere ikerketan laguntzeko erabiltzen baitzuten.
 Agindua eman bezain laster bete denez, ez dakit zer gertatu zaien bertan zeuden beleei...
 Oraingoz, ate guztiak zigilatu dira, eta burutu gabe zeuden bertako lan-aginduak eskuz itxi dira.
@@ -29849,7 +29849,7 @@
       <c r="G426" s="9" t="str">
         <f aca="false">IF(ISBLANK(C426),E426,C426)</f>
         <v>Honek segari baten eguneroko abandonatua dirudi:
-“Ate ireki batzuk deskonektatzeko agindu digute, energia gainkarga ezohikoa antzeman zen ingurukoak dira.
+“Ate ireki batzuk deskonektatzeko agindu digute. Energia gainkarga ezohikoa antzeman zen ingurukoak dira.
 Zonalde hori nahiko aktiboa zen lehen, Komisioko kideek &lt;i&gt;sorgina&lt;/i&gt; bere ikerketan laguntzeko erabiltzen baitzuten.
 Agindua eman bezain laster bete denez, ez dakit zer gertatu zaien bertan zeuden beleei...
 Oraingoz, ate guztiak zigilatu dira, eta burutu gabe zeuden bertako lan-aginduak eskuz itxi dira.
@@ -31127,12 +31127,12 @@
       </c>
       <c r="F469" s="9" t="str">
         <f aca="false">IF(ISBLANK(C469),D469,C469)</f>
-        <v>Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia, zu arrautza zinen garaia baino zaharragoa da.
+        <v>Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia da, zu arrautza zinen garaia baino zaharragoa.
 Badirudi sorginak kendu beharra izan zuela, gorputza etengabe puzten ari zitzaiolako. Hori ere zure garaia igarota bizitzen jarraitzearen ondorioetako bat da.</v>
       </c>
       <c r="G469" s="9" t="str">
         <f aca="false">IF(ISBLANK(C469),E469,C469)</f>
-        <v>Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia, zu arrautza zinen garaia baino zaharragoa da.
+        <v>Eraztun honen jabea Errautsontzi sorgina zen. Bere senarra zenaren oparia da, zu arrautza zinen garaia baino zaharragoa.
 Badirudi sorginak kendu beharra izan zuela, gorputza etengabe puzten ari zitzaiolako. Hori ere zure garaia igarota bizitzen jarraitzearen ondorioetako bat da.</v>
       </c>
       <c r="H469" s="5"/>
@@ -32157,12 +32157,12 @@
       </c>
       <c r="F505" s="9" t="str">
         <f aca="false">IF(ISBLANK(C505),D505,C505)</f>
-        <v>Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere Oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
+        <v>Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere, oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
 Esku egokietan, instrumentu honek naturarekin elkarrizketa bat sor dezake, inguruko landaretza nolabait kontrolatzea ahalbidetuz.</v>
       </c>
       <c r="G505" s="9" t="str">
         <f aca="false">IF(ISBLANK(C505),E505,C505)</f>
-        <v>Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere Oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
+        <v>Adarra instrumentu maitatua da oihaneko biztanleen artean, izan ere, oihaneko oihartzun sakonekin harmonizatzeko gaitasuna dauka.
 Esku egokietan, instrumentu honek naturarekin elkarrizketa bat sor dezake, inguruko landaretza nolabait kontrolatzea ahalbidetuz.</v>
       </c>
       <c r="H505" s="5"/>
@@ -32498,14 +32498,14 @@
       <c r="F517" s="9" t="str">
         <f aca="false">IF(ISBLANK(C517),D517,C517)</f>
         <v>Eskalara egindako atearen maketa honek ohar bat dauka itsatsita:
-&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrak bezala.
+&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrekoek bezala.
 Ganbera korazatu bat aurkeztuko dugu, ate berrientzako argindar-sarea elikatzeko arimak prozesatuko dituena.
 Guztia Komisioak automatizatua egongo da, erosketak egiteko erabiltzen diren arima txikiak ere sistema berrelikatzeko erabiliko dira.”&lt;/i&gt;</v>
       </c>
       <c r="G517" s="9" t="str">
         <f aca="false">IF(ISBLANK(C517),E517,C517)</f>
         <v>Eskalara egindako atearen maketa honek ohar bat dauka itsatsita:
-&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrak bezala.
+&lt;i&gt;”Finagoak dira, erabilerrazagoak, eta fidagarriagoak. Dagoeneko ez dituzte arima gordinak prozesatzen, diseinu zaharrekoek bezala.
 Ganbera korazatu bat aurkeztuko dugu, ate berrientzako argindar-sarea elikatzeko arimak prozesatuko dituena.
 Guztia Komisioak automatizatua egongo da, erosketak egiteko erabiltzen diren arima txikiak ere sistema berrelikatzeko erabiliko dira.”&lt;/i&gt;</v>
       </c>

</xml_diff>